<commit_message>
Enhanced RetryAnalyzer with custom annotation. Refactored app pom (all item search result pages will be Catalog type). Renamed all test classes to start with Test, as per required by TestNG, and also best practice
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\IdeaProjects\winterweekendselenium\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FAB92B-8EC5-40F3-8A4C-F1EDDEB92F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB509949-F276-445E-B212-C6E8742CFDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{737F456A-BA07-46AB-AAA2-7DD47C4B7DA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{737F456A-BA07-46AB-AAA2-7DD47C4B7DA6}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginValidEmailInvalidPass" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginInvalidEmailValidPass" sheetId="2" r:id="rId2"/>
+    <sheet name="testAddItemToCart" sheetId="3" r:id="rId1"/>
+    <sheet name="LoginValidEmailInvalidPass" sheetId="1" r:id="rId2"/>
+    <sheet name="LoginInvalidEmailValidPass" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>User</t>
   </si>
@@ -111,6 +112,12 @@
   </si>
   <si>
     <t>aghilesham20@yahoo.cm</t>
+  </si>
+  <si>
+    <t>expected_message</t>
+  </si>
+  <si>
+    <t>Product successfully added to your shopping cart</t>
   </si>
 </sst>
 </file>
@@ -475,10 +482,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B85C5A3-78B0-461E-A595-82D47752DD98}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DD4A45-1385-4380-889D-88CF15B37225}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -584,7 +616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620C28E2-708E-44BB-B761-63885062F8E9}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>